<commit_message>
Update presentation. Try out 3d plot
</commit_message>
<xml_diff>
--- a/Compare_K_Hclust/compare_clusters.xlsx
+++ b/Compare_K_Hclust/compare_clusters.xlsx
@@ -5543,7 +5543,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -5551,7 +5551,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -5559,7 +5559,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>203</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -5567,7 +5567,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>205</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -5575,7 +5575,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -5583,7 +5583,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -5599,7 +5599,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -5607,7 +5607,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>214</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -5623,7 +5623,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>216</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>217</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -5639,7 +5639,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -5647,7 +5647,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
@@ -5655,7 +5655,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -5663,7 +5663,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
@@ -5671,7 +5671,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>215</v>
+        <v>21</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
@@ -5679,7 +5679,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>228</v>
       </c>
       <c r="B19" t="n">
         <v>1</v>
@@ -5687,7 +5687,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>230</v>
       </c>
       <c r="B20" t="n">
         <v>1</v>
@@ -5695,7 +5695,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>1</v>
@@ -5703,7 +5703,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>233</v>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -5719,7 +5719,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="B24" t="n">
         <v>1</v>
@@ -5727,7 +5727,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
@@ -5735,7 +5735,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="B26" t="n">
         <v>1</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -5751,7 +5751,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>241</v>
       </c>
       <c r="B28" t="n">
         <v>1</v>
@@ -5759,7 +5759,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B29" t="n">
         <v>1</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="B30" t="n">
         <v>1</v>
@@ -5775,7 +5775,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
@@ -5783,7 +5783,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>246</v>
       </c>
       <c r="B32" t="n">
         <v>1</v>
@@ -5791,7 +5791,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>247</v>
       </c>
       <c r="B33" t="n">
         <v>1</v>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>248</v>
       </c>
       <c r="B34" t="n">
         <v>1</v>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="B35" t="n">
         <v>1</v>
@@ -5815,7 +5815,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>251</v>
       </c>
       <c r="B36" t="n">
         <v>1</v>
@@ -5823,7 +5823,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="B37" t="n">
         <v>1</v>
@@ -5831,7 +5831,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="B38" t="n">
         <v>1</v>
@@ -5839,7 +5839,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>257</v>
       </c>
       <c r="B39" t="n">
         <v>1</v>
@@ -5847,7 +5847,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>258</v>
       </c>
       <c r="B40" t="n">
         <v>1</v>
@@ -5855,7 +5855,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>259</v>
       </c>
       <c r="B41" t="n">
         <v>1</v>
@@ -5863,7 +5863,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>234</v>
+        <v>59</v>
       </c>
       <c r="B42" t="n">
         <v>1</v>
@@ -5871,7 +5871,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="B43" t="n">
         <v>1</v>
@@ -5879,7 +5879,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>263</v>
       </c>
       <c r="B44" t="n">
         <v>1</v>
@@ -5887,7 +5887,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
@@ -5895,7 +5895,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="B46" t="n">
         <v>1</v>
@@ -5903,7 +5903,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="B47" t="n">
         <v>1</v>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>266</v>
       </c>
       <c r="B48" t="n">
         <v>1</v>
@@ -5919,7 +5919,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>268</v>
       </c>
       <c r="B49" t="n">
         <v>1</v>
@@ -5927,7 +5927,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B50" t="n">
         <v>1</v>
@@ -5935,7 +5935,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="B51" t="n">
         <v>1</v>
@@ -5943,7 +5943,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>270</v>
       </c>
       <c r="B52" t="n">
         <v>1</v>
@@ -5951,7 +5951,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>271</v>
       </c>
       <c r="B53" t="n">
         <v>1</v>
@@ -5959,7 +5959,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>272</v>
       </c>
       <c r="B54" t="n">
         <v>1</v>
@@ -5967,7 +5967,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>273</v>
       </c>
       <c r="B55" t="n">
         <v>1</v>
@@ -5975,7 +5975,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>274</v>
       </c>
       <c r="B56" t="n">
         <v>1</v>
@@ -5983,7 +5983,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
       <c r="B57" t="n">
         <v>1</v>
@@ -5991,7 +5991,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>278</v>
       </c>
       <c r="B58" t="n">
         <v>1</v>
@@ -5999,7 +5999,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>77</v>
       </c>
       <c r="B59" t="n">
         <v>1</v>
@@ -6007,7 +6007,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>279</v>
       </c>
       <c r="B60" t="n">
         <v>1</v>
@@ -6015,7 +6015,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>280</v>
       </c>
       <c r="B61" t="n">
         <v>1</v>
@@ -6023,7 +6023,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>281</v>
       </c>
       <c r="B62" t="n">
         <v>1</v>
@@ -6031,7 +6031,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>282</v>
       </c>
       <c r="B63" t="n">
         <v>1</v>
@@ -6039,7 +6039,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>283</v>
       </c>
       <c r="B64" t="n">
         <v>1</v>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>250</v>
+        <v>284</v>
       </c>
       <c r="B65" t="n">
         <v>1</v>
@@ -6055,7 +6055,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="B66" t="n">
         <v>1</v>
@@ -6063,7 +6063,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>50</v>
+        <v>286</v>
       </c>
       <c r="B67" t="n">
         <v>1</v>
@@ -6071,7 +6071,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>252</v>
+        <v>287</v>
       </c>
       <c r="B68" t="n">
         <v>1</v>
@@ -6079,7 +6079,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>289</v>
       </c>
       <c r="B69" t="n">
         <v>1</v>
@@ -6087,7 +6087,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="B70" t="n">
         <v>1</v>
@@ -6095,7 +6095,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>291</v>
       </c>
       <c r="B71" t="n">
         <v>1</v>
@@ -6103,7 +6103,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>292</v>
       </c>
       <c r="B72" t="n">
         <v>1</v>
@@ -6111,7 +6111,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>295</v>
       </c>
       <c r="B73" t="n">
         <v>1</v>
@@ -6119,7 +6119,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>254</v>
+        <v>296</v>
       </c>
       <c r="B74" t="n">
         <v>1</v>
@@ -6127,7 +6127,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="B75" t="n">
         <v>1</v>
@@ -6135,7 +6135,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>298</v>
       </c>
       <c r="B76" t="n">
         <v>1</v>
@@ -6143,7 +6143,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>299</v>
       </c>
       <c r="B77" t="n">
         <v>1</v>
@@ -6151,7 +6151,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="B78" t="n">
         <v>1</v>
@@ -6159,7 +6159,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>304</v>
       </c>
       <c r="B79" t="n">
         <v>1</v>
@@ -6167,7 +6167,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>261</v>
+        <v>306</v>
       </c>
       <c r="B80" t="n">
         <v>1</v>
@@ -6175,7 +6175,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>60</v>
+        <v>308</v>
       </c>
       <c r="B81" t="n">
         <v>1</v>
@@ -6183,7 +6183,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B82" t="n">
         <v>1</v>
@@ -6191,7 +6191,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>62</v>
+        <v>311</v>
       </c>
       <c r="B83" t="n">
         <v>1</v>
@@ -6199,7 +6199,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>63</v>
+        <v>312</v>
       </c>
       <c r="B84" t="n">
         <v>1</v>
@@ -6207,7 +6207,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B85" t="n">
         <v>1</v>
@@ -6215,7 +6215,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>65</v>
+        <v>314</v>
       </c>
       <c r="B86" t="n">
         <v>1</v>
@@ -6223,7 +6223,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="B87" t="n">
         <v>1</v>
@@ -6231,7 +6231,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>67</v>
+        <v>319</v>
       </c>
       <c r="B88" t="n">
         <v>1</v>
@@ -6239,7 +6239,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="B89" t="n">
         <v>1</v>
@@ -6247,7 +6247,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>321</v>
       </c>
       <c r="B90" t="n">
         <v>1</v>
@@ -6255,7 +6255,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>267</v>
+        <v>324</v>
       </c>
       <c r="B91" t="n">
         <v>1</v>
@@ -6263,7 +6263,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>71</v>
+        <v>325</v>
       </c>
       <c r="B92" t="n">
         <v>1</v>
@@ -6271,7 +6271,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="B93" t="n">
         <v>1</v>
@@ -6279,7 +6279,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="B94" t="n">
         <v>1</v>
@@ -6287,7 +6287,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>73</v>
+        <v>328</v>
       </c>
       <c r="B95" t="n">
         <v>1</v>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B96" t="n">
         <v>1</v>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>75</v>
+        <v>329</v>
       </c>
       <c r="B97" t="n">
         <v>1</v>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>76</v>
+        <v>330</v>
       </c>
       <c r="B98" t="n">
         <v>1</v>
@@ -6319,7 +6319,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>78</v>
+        <v>331</v>
       </c>
       <c r="B99" t="n">
         <v>1</v>
@@ -6327,7 +6327,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>332</v>
       </c>
       <c r="B100" t="n">
         <v>1</v>
@@ -6335,7 +6335,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B101" t="n">
         <v>1</v>
@@ -6343,7 +6343,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>81</v>
+        <v>333</v>
       </c>
       <c r="B102" t="n">
         <v>1</v>
@@ -6351,7 +6351,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>82</v>
+        <v>334</v>
       </c>
       <c r="B103" t="n">
         <v>1</v>
@@ -6359,7 +6359,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>335</v>
       </c>
       <c r="B104" t="n">
         <v>1</v>
@@ -6367,7 +6367,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>293</v>
+        <v>336</v>
       </c>
       <c r="B105" t="n">
         <v>1</v>
@@ -6375,7 +6375,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>294</v>
+        <v>337</v>
       </c>
       <c r="B106" t="n">
         <v>1</v>
@@ -6383,7 +6383,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>83</v>
+        <v>339</v>
       </c>
       <c r="B107" t="n">
         <v>1</v>
@@ -6391,7 +6391,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>84</v>
+        <v>341</v>
       </c>
       <c r="B108" t="n">
         <v>1</v>
@@ -6399,7 +6399,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>85</v>
+        <v>342</v>
       </c>
       <c r="B109" t="n">
         <v>1</v>
@@ -6407,7 +6407,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>343</v>
       </c>
       <c r="B110" t="n">
         <v>1</v>
@@ -6415,7 +6415,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="B111" t="n">
         <v>1</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>301</v>
+        <v>346</v>
       </c>
       <c r="B112" t="n">
         <v>1</v>
@@ -6431,7 +6431,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>87</v>
+        <v>347</v>
       </c>
       <c r="B113" t="n">
         <v>1</v>
@@ -6439,7 +6439,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>88</v>
+        <v>348</v>
       </c>
       <c r="B114" t="n">
         <v>1</v>
@@ -6447,7 +6447,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>303</v>
+        <v>349</v>
       </c>
       <c r="B115" t="n">
         <v>1</v>
@@ -6455,7 +6455,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>89</v>
+        <v>351</v>
       </c>
       <c r="B116" t="n">
         <v>1</v>
@@ -6463,7 +6463,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>305</v>
+        <v>352</v>
       </c>
       <c r="B117" t="n">
         <v>1</v>
@@ -6471,7 +6471,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>353</v>
       </c>
       <c r="B118" t="n">
         <v>1</v>
@@ -6479,7 +6479,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>307</v>
+        <v>354</v>
       </c>
       <c r="B119" t="n">
         <v>1</v>
@@ -6487,7 +6487,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>91</v>
+        <v>355</v>
       </c>
       <c r="B120" t="n">
         <v>1</v>
@@ -6495,7 +6495,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>93</v>
+        <v>356</v>
       </c>
       <c r="B121" t="n">
         <v>1</v>
@@ -6503,7 +6503,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>309</v>
+        <v>124</v>
       </c>
       <c r="B122" t="n">
         <v>1</v>
@@ -6511,7 +6511,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>310</v>
+        <v>128</v>
       </c>
       <c r="B123" t="n">
         <v>1</v>
@@ -6519,7 +6519,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>313</v>
+        <v>357</v>
       </c>
       <c r="B124" t="n">
         <v>1</v>
@@ -6527,7 +6527,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="B125" t="n">
         <v>1</v>
@@ -6535,7 +6535,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>316</v>
+        <v>131</v>
       </c>
       <c r="B126" t="n">
         <v>1</v>
@@ -6543,7 +6543,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>96</v>
+        <v>362</v>
       </c>
       <c r="B127" t="n">
         <v>1</v>
@@ -6551,7 +6551,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>97</v>
+        <v>363</v>
       </c>
       <c r="B128" t="n">
         <v>1</v>
@@ -6559,7 +6559,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>98</v>
+        <v>364</v>
       </c>
       <c r="B129" t="n">
         <v>1</v>
@@ -6567,7 +6567,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>317</v>
+        <v>366</v>
       </c>
       <c r="B130" t="n">
         <v>1</v>
@@ -6575,7 +6575,7 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>318</v>
+        <v>368</v>
       </c>
       <c r="B131" t="n">
         <v>1</v>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>99</v>
+        <v>369</v>
       </c>
       <c r="B132" t="n">
         <v>1</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>100</v>
+        <v>370</v>
       </c>
       <c r="B133" t="n">
         <v>1</v>
@@ -6599,7 +6599,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="B134" t="n">
         <v>1</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>102</v>
+        <v>372</v>
       </c>
       <c r="B135" t="n">
         <v>1</v>
@@ -6615,7 +6615,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>322</v>
+        <v>373</v>
       </c>
       <c r="B136" t="n">
         <v>1</v>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>323</v>
+        <v>374</v>
       </c>
       <c r="B137" t="n">
         <v>1</v>
@@ -6631,7 +6631,7 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>103</v>
+        <v>376</v>
       </c>
       <c r="B138" t="n">
         <v>1</v>
@@ -6639,7 +6639,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>104</v>
+        <v>377</v>
       </c>
       <c r="B139" t="n">
         <v>1</v>
@@ -6647,7 +6647,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="B140" t="n">
         <v>1</v>
@@ -6655,7 +6655,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>107</v>
+        <v>380</v>
       </c>
       <c r="B141" t="n">
         <v>1</v>
@@ -6663,7 +6663,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>108</v>
+        <v>381</v>
       </c>
       <c r="B142" t="n">
         <v>1</v>
@@ -6671,7 +6671,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>110</v>
+        <v>383</v>
       </c>
       <c r="B143" t="n">
         <v>1</v>
@@ -6679,7 +6679,7 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="B144" t="n">
         <v>1</v>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>112</v>
+        <v>384</v>
       </c>
       <c r="B145" t="n">
         <v>1</v>
@@ -6695,7 +6695,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>338</v>
+        <v>385</v>
       </c>
       <c r="B146" t="n">
         <v>1</v>
@@ -6703,7 +6703,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>113</v>
+        <v>387</v>
       </c>
       <c r="B147" t="n">
         <v>1</v>
@@ -6711,7 +6711,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>340</v>
+        <v>389</v>
       </c>
       <c r="B148" t="n">
         <v>1</v>
@@ -6719,7 +6719,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>114</v>
+        <v>390</v>
       </c>
       <c r="B149" t="n">
         <v>1</v>
@@ -6727,7 +6727,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>115</v>
+        <v>391</v>
       </c>
       <c r="B150" t="n">
         <v>1</v>
@@ -6735,7 +6735,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>344</v>
+        <v>146</v>
       </c>
       <c r="B151" t="n">
         <v>1</v>
@@ -6743,7 +6743,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>116</v>
+        <v>395</v>
       </c>
       <c r="B152" t="n">
         <v>1</v>
@@ -6751,7 +6751,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>117</v>
+        <v>396</v>
       </c>
       <c r="B153" t="n">
         <v>1</v>
@@ -6759,7 +6759,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="B154" t="n">
         <v>1</v>
@@ -6767,7 +6767,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>119</v>
+        <v>397</v>
       </c>
       <c r="B155" t="n">
         <v>1</v>
@@ -6775,7 +6775,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>120</v>
+        <v>400</v>
       </c>
       <c r="B156" t="n">
         <v>1</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>350</v>
+        <v>402</v>
       </c>
       <c r="B157" t="n">
         <v>1</v>
@@ -6791,7 +6791,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>121</v>
+        <v>403</v>
       </c>
       <c r="B158" t="n">
         <v>1</v>
@@ -6799,7 +6799,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="B159" t="n">
         <v>1</v>
@@ -6807,7 +6807,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>123</v>
+        <v>407</v>
       </c>
       <c r="B160" t="n">
         <v>1</v>
@@ -6815,7 +6815,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>125</v>
+        <v>411</v>
       </c>
       <c r="B161" t="n">
         <v>1</v>
@@ -6823,7 +6823,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B162" t="n">
         <v>1</v>
@@ -6831,7 +6831,7 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B163" t="n">
         <v>1</v>
@@ -6839,7 +6839,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>129</v>
+        <v>412</v>
       </c>
       <c r="B164" t="n">
         <v>1</v>
@@ -6847,7 +6847,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>358</v>
+        <v>413</v>
       </c>
       <c r="B165" t="n">
         <v>1</v>
@@ -6855,7 +6855,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>359</v>
+        <v>414</v>
       </c>
       <c r="B166" t="n">
         <v>1</v>
@@ -6863,7 +6863,7 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>130</v>
+        <v>415</v>
       </c>
       <c r="B167" t="n">
         <v>1</v>
@@ -6871,7 +6871,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>361</v>
+        <v>416</v>
       </c>
       <c r="B168" t="n">
         <v>1</v>
@@ -6879,7 +6879,7 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>365</v>
+        <v>417</v>
       </c>
       <c r="B169" t="n">
         <v>1</v>
@@ -6887,7 +6887,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>367</v>
+        <v>159</v>
       </c>
       <c r="B170" t="n">
         <v>1</v>
@@ -6895,7 +6895,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>371</v>
+        <v>418</v>
       </c>
       <c r="B171" t="n">
         <v>1</v>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="B172" t="n">
         <v>1</v>
@@ -6911,7 +6911,7 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>134</v>
+        <v>421</v>
       </c>
       <c r="B173" t="n">
         <v>1</v>
@@ -6919,7 +6919,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>375</v>
+        <v>422</v>
       </c>
       <c r="B174" t="n">
         <v>1</v>
@@ -6927,7 +6927,7 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>378</v>
+        <v>423</v>
       </c>
       <c r="B175" t="n">
         <v>1</v>
@@ -6935,7 +6935,7 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>379</v>
+        <v>424</v>
       </c>
       <c r="B176" t="n">
         <v>1</v>
@@ -6943,7 +6943,7 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>382</v>
+        <v>425</v>
       </c>
       <c r="B177" t="n">
         <v>1</v>
@@ -6951,7 +6951,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>136</v>
+        <v>426</v>
       </c>
       <c r="B178" t="n">
         <v>1</v>
@@ -6959,7 +6959,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>137</v>
+        <v>427</v>
       </c>
       <c r="B179" t="n">
         <v>1</v>
@@ -6967,7 +6967,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>138</v>
+        <v>428</v>
       </c>
       <c r="B180" t="n">
         <v>1</v>
@@ -6975,7 +6975,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>139</v>
+        <v>429</v>
       </c>
       <c r="B181" t="n">
         <v>1</v>
@@ -6983,7 +6983,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="B182" t="n">
         <v>1</v>
@@ -6991,7 +6991,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>142</v>
+        <v>430</v>
       </c>
       <c r="B183" t="n">
         <v>1</v>
@@ -6999,7 +6999,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>386</v>
+        <v>433</v>
       </c>
       <c r="B184" t="n">
         <v>1</v>
@@ -7007,7 +7007,7 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>388</v>
+        <v>171</v>
       </c>
       <c r="B185" t="n">
         <v>1</v>
@@ -7015,7 +7015,7 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>143</v>
+        <v>438</v>
       </c>
       <c r="B186" t="n">
         <v>1</v>
@@ -7023,7 +7023,7 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>144</v>
+        <v>439</v>
       </c>
       <c r="B187" t="n">
         <v>1</v>
@@ -7031,7 +7031,7 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>145</v>
+        <v>440</v>
       </c>
       <c r="B188" t="n">
         <v>1</v>
@@ -7039,7 +7039,7 @@
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>392</v>
+        <v>441</v>
       </c>
       <c r="B189" t="n">
         <v>1</v>
@@ -7047,7 +7047,7 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="B190" t="n">
         <v>1</v>
@@ -7055,7 +7055,7 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>394</v>
+        <v>180</v>
       </c>
       <c r="B191" t="n">
         <v>1</v>
@@ -7063,7 +7063,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>398</v>
+        <v>187</v>
       </c>
       <c r="B192" t="n">
         <v>1</v>
@@ -7071,7 +7071,7 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>148</v>
+        <v>445</v>
       </c>
       <c r="B193" t="n">
         <v>1</v>
@@ -7079,7 +7079,7 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>399</v>
+        <v>447</v>
       </c>
       <c r="B194" t="n">
         <v>1</v>
@@ -7087,7 +7087,7 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>401</v>
+        <v>448</v>
       </c>
       <c r="B195" t="n">
         <v>1</v>
@@ -7095,7 +7095,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>404</v>
+        <v>449</v>
       </c>
       <c r="B196" t="n">
         <v>1</v>
@@ -7103,7 +7103,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>405</v>
+        <v>450</v>
       </c>
       <c r="B197" t="n">
         <v>1</v>
@@ -7111,7 +7111,7 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>406</v>
+        <v>451</v>
       </c>
       <c r="B198" t="n">
         <v>1</v>
@@ -7119,7 +7119,7 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>150</v>
+        <v>452</v>
       </c>
       <c r="B199" t="n">
         <v>1</v>
@@ -7127,7 +7127,7 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>408</v>
+        <v>455</v>
       </c>
       <c r="B200" t="n">
         <v>1</v>
@@ -7135,7 +7135,7 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>409</v>
+        <v>457</v>
       </c>
       <c r="B201" t="n">
         <v>1</v>
@@ -7143,7 +7143,7 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="B202" t="n">
         <v>1</v>
@@ -7151,7 +7151,7 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>410</v>
+        <v>458</v>
       </c>
       <c r="B203" t="n">
         <v>1</v>
@@ -7159,7 +7159,7 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>153</v>
+        <v>459</v>
       </c>
       <c r="B204" t="n">
         <v>1</v>
@@ -7167,7 +7167,7 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>155</v>
+        <v>461</v>
       </c>
       <c r="B205" t="n">
         <v>1</v>
@@ -7175,7 +7175,7 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>156</v>
+        <v>462</v>
       </c>
       <c r="B206" t="n">
         <v>1</v>
@@ -7183,7 +7183,7 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>157</v>
+        <v>463</v>
       </c>
       <c r="B207" t="n">
         <v>1</v>
@@ -7191,433 +7191,9 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>158</v>
+        <v>464</v>
       </c>
       <c r="B208" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="s">
-        <v>161</v>
-      </c>
-      <c r="B209" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="s">
-        <v>419</v>
-      </c>
-      <c r="B210" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="s">
-        <v>420</v>
-      </c>
-      <c r="B211" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="s">
-        <v>162</v>
-      </c>
-      <c r="B212" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="s">
-        <v>163</v>
-      </c>
-      <c r="B213" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="s">
-        <v>164</v>
-      </c>
-      <c r="B214" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="s">
-        <v>165</v>
-      </c>
-      <c r="B215" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="s">
-        <v>166</v>
-      </c>
-      <c r="B216" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="s">
-        <v>168</v>
-      </c>
-      <c r="B217" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="s">
-        <v>431</v>
-      </c>
-      <c r="B218" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="s">
-        <v>432</v>
-      </c>
-      <c r="B219" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="s">
-        <v>169</v>
-      </c>
-      <c r="B220" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="s">
-        <v>434</v>
-      </c>
-      <c r="B221" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="s">
-        <v>170</v>
-      </c>
-      <c r="B222" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="s">
-        <v>435</v>
-      </c>
-      <c r="B223" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="s">
-        <v>172</v>
-      </c>
-      <c r="B224" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="s">
-        <v>173</v>
-      </c>
-      <c r="B225" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="s">
-        <v>436</v>
-      </c>
-      <c r="B226" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="s">
-        <v>174</v>
-      </c>
-      <c r="B227" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="s">
-        <v>437</v>
-      </c>
-      <c r="B228" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="s">
-        <v>175</v>
-      </c>
-      <c r="B229" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="s">
-        <v>176</v>
-      </c>
-      <c r="B230" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="s">
-        <v>177</v>
-      </c>
-      <c r="B231" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="s">
-        <v>178</v>
-      </c>
-      <c r="B232" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="s">
-        <v>179</v>
-      </c>
-      <c r="B233" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="s">
-        <v>181</v>
-      </c>
-      <c r="B234" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="s">
-        <v>182</v>
-      </c>
-      <c r="B235" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="s">
-        <v>183</v>
-      </c>
-      <c r="B236" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="s">
-        <v>184</v>
-      </c>
-      <c r="B237" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="s">
-        <v>443</v>
-      </c>
-      <c r="B238" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="s">
-        <v>185</v>
-      </c>
-      <c r="B239" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="s">
-        <v>444</v>
-      </c>
-      <c r="B240" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="s">
-        <v>186</v>
-      </c>
-      <c r="B241" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="s">
-        <v>446</v>
-      </c>
-      <c r="B242" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="s">
-        <v>453</v>
-      </c>
-      <c r="B243" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="s">
-        <v>454</v>
-      </c>
-      <c r="B244" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="s">
-        <v>456</v>
-      </c>
-      <c r="B245" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="s">
-        <v>189</v>
-      </c>
-      <c r="B246" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="s">
-        <v>460</v>
-      </c>
-      <c r="B247" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="s">
-        <v>190</v>
-      </c>
-      <c r="B248" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="s">
-        <v>191</v>
-      </c>
-      <c r="B249" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="s">
-        <v>192</v>
-      </c>
-      <c r="B250" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="s">
-        <v>193</v>
-      </c>
-      <c r="B251" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="s">
-        <v>194</v>
-      </c>
-      <c r="B252" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="s">
-        <v>195</v>
-      </c>
-      <c r="B253" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="s">
-        <v>196</v>
-      </c>
-      <c r="B254" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="s">
-        <v>197</v>
-      </c>
-      <c r="B255" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="s">
-        <v>465</v>
-      </c>
-      <c r="B256" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="s">
-        <v>466</v>
-      </c>
-      <c r="B257" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="s">
-        <v>467</v>
-      </c>
-      <c r="B258" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="s">
-        <v>198</v>
-      </c>
-      <c r="B259" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="s">
-        <v>199</v>
-      </c>
-      <c r="B260" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="s">
-        <v>468</v>
-      </c>
-      <c r="B261" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7645,7 +7221,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
@@ -7653,7 +7229,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
@@ -7661,7 +7237,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
@@ -7669,7 +7245,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
@@ -7677,7 +7253,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -7685,7 +7261,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
@@ -7693,7 +7269,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -7701,7 +7277,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>2</v>
@@ -7709,7 +7285,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>2</v>
@@ -7717,7 +7293,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>2</v>
@@ -7725,7 +7301,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>2</v>
@@ -7733,7 +7309,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>2</v>
@@ -7741,7 +7317,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B14" t="n">
         <v>2</v>
@@ -7749,7 +7325,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B15" t="n">
         <v>2</v>
@@ -7757,7 +7333,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>226</v>
+        <v>12</v>
       </c>
       <c r="B16" t="n">
         <v>2</v>
@@ -7765,7 +7341,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B17" t="n">
         <v>2</v>
@@ -7773,7 +7349,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>215</v>
       </c>
       <c r="B18" t="n">
         <v>2</v>
@@ -7781,7 +7357,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>13</v>
       </c>
       <c r="B19" t="n">
         <v>2</v>
@@ -7789,7 +7365,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>14</v>
       </c>
       <c r="B20" t="n">
         <v>2</v>
@@ -7797,7 +7373,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B21" t="n">
         <v>2</v>
@@ -7805,7 +7381,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="B22" t="n">
         <v>2</v>
@@ -7813,7 +7389,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>16</v>
       </c>
       <c r="B23" t="n">
         <v>2</v>
@@ -7821,7 +7397,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="B24" t="n">
         <v>2</v>
@@ -7829,7 +7405,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>221</v>
       </c>
       <c r="B25" t="n">
         <v>2</v>
@@ -7837,7 +7413,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
@@ -7845,7 +7421,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B27" t="n">
         <v>2</v>
@@ -7853,7 +7429,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>241</v>
+        <v>18</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
@@ -7861,7 +7437,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B29" t="n">
         <v>2</v>
@@ -7869,7 +7445,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="B30" t="n">
         <v>2</v>
@@ -7877,7 +7453,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B31" t="n">
         <v>2</v>
@@ -7885,7 +7461,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>246</v>
+        <v>20</v>
       </c>
       <c r="B32" t="n">
         <v>2</v>
@@ -7893,7 +7469,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>247</v>
+        <v>22</v>
       </c>
       <c r="B33" t="n">
         <v>2</v>
@@ -7901,7 +7477,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>248</v>
+        <v>23</v>
       </c>
       <c r="B34" t="n">
         <v>2</v>
@@ -7909,7 +7485,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B35" t="n">
         <v>2</v>
@@ -7917,7 +7493,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>251</v>
+        <v>24</v>
       </c>
       <c r="B36" t="n">
         <v>2</v>
@@ -7925,7 +7501,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>255</v>
+        <v>25</v>
       </c>
       <c r="B37" t="n">
         <v>2</v>
@@ -7933,7 +7509,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="B38" t="n">
         <v>2</v>
@@ -7941,7 +7517,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>257</v>
+        <v>27</v>
       </c>
       <c r="B39" t="n">
         <v>2</v>
@@ -7949,7 +7525,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>258</v>
+        <v>28</v>
       </c>
       <c r="B40" t="n">
         <v>2</v>
@@ -7957,7 +7533,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="B41" t="n">
         <v>2</v>
@@ -7965,7 +7541,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>234</v>
       </c>
       <c r="B42" t="n">
         <v>2</v>
@@ -7973,7 +7549,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="B43" t="n">
         <v>2</v>
@@ -7981,7 +7557,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>263</v>
+        <v>30</v>
       </c>
       <c r="B44" t="n">
         <v>2</v>
@@ -7989,7 +7565,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="B45" t="n">
         <v>2</v>
@@ -7997,7 +7573,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="B46" t="n">
         <v>2</v>
@@ -8005,7 +7581,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="B47" t="n">
         <v>2</v>
@@ -8013,7 +7589,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>266</v>
+        <v>32</v>
       </c>
       <c r="B48" t="n">
         <v>2</v>
@@ -8021,7 +7597,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>268</v>
+        <v>33</v>
       </c>
       <c r="B49" t="n">
         <v>2</v>
@@ -8029,7 +7605,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B50" t="n">
         <v>2</v>
@@ -8037,7 +7613,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="B51" t="n">
         <v>2</v>
@@ -8045,7 +7621,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>270</v>
+        <v>36</v>
       </c>
       <c r="B52" t="n">
         <v>2</v>
@@ -8053,7 +7629,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>271</v>
+        <v>37</v>
       </c>
       <c r="B53" t="n">
         <v>2</v>
@@ -8061,7 +7637,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>272</v>
+        <v>40</v>
       </c>
       <c r="B54" t="n">
         <v>2</v>
@@ -8069,7 +7645,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>273</v>
+        <v>41</v>
       </c>
       <c r="B55" t="n">
         <v>2</v>
@@ -8077,7 +7653,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>274</v>
+        <v>42</v>
       </c>
       <c r="B56" t="n">
         <v>2</v>
@@ -8085,7 +7661,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="B57" t="n">
         <v>2</v>
@@ -8093,7 +7669,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>278</v>
+        <v>43</v>
       </c>
       <c r="B58" t="n">
         <v>2</v>
@@ -8101,7 +7677,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>245</v>
       </c>
       <c r="B59" t="n">
         <v>2</v>
@@ -8109,7 +7685,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>279</v>
+        <v>44</v>
       </c>
       <c r="B60" t="n">
         <v>2</v>
@@ -8117,7 +7693,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="B61" t="n">
         <v>2</v>
@@ -8125,7 +7701,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>281</v>
+        <v>46</v>
       </c>
       <c r="B62" t="n">
         <v>2</v>
@@ -8133,7 +7709,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>282</v>
+        <v>47</v>
       </c>
       <c r="B63" t="n">
         <v>2</v>
@@ -8141,7 +7717,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>283</v>
+        <v>48</v>
       </c>
       <c r="B64" t="n">
         <v>2</v>
@@ -8149,7 +7725,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="B65" t="n">
         <v>2</v>
@@ -8157,7 +7733,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>285</v>
+        <v>49</v>
       </c>
       <c r="B66" t="n">
         <v>2</v>
@@ -8165,7 +7741,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>286</v>
+        <v>50</v>
       </c>
       <c r="B67" t="n">
         <v>2</v>
@@ -8173,7 +7749,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="B68" t="n">
         <v>2</v>
@@ -8181,7 +7757,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>289</v>
+        <v>51</v>
       </c>
       <c r="B69" t="n">
         <v>2</v>
@@ -8189,7 +7765,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="B70" t="n">
         <v>2</v>
@@ -8197,7 +7773,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>291</v>
+        <v>52</v>
       </c>
       <c r="B71" t="n">
         <v>2</v>
@@ -8205,7 +7781,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>53</v>
       </c>
       <c r="B72" t="n">
         <v>2</v>
@@ -8213,7 +7789,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>295</v>
+        <v>54</v>
       </c>
       <c r="B73" t="n">
         <v>2</v>
@@ -8221,7 +7797,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>296</v>
+        <v>254</v>
       </c>
       <c r="B74" t="n">
         <v>2</v>
@@ -8229,7 +7805,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>55</v>
       </c>
       <c r="B75" t="n">
         <v>2</v>
@@ -8237,7 +7813,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>298</v>
+        <v>56</v>
       </c>
       <c r="B76" t="n">
         <v>2</v>
@@ -8245,7 +7821,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>299</v>
+        <v>57</v>
       </c>
       <c r="B77" t="n">
         <v>2</v>
@@ -8253,7 +7829,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>302</v>
+        <v>260</v>
       </c>
       <c r="B78" t="n">
         <v>2</v>
@@ -8261,7 +7837,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>304</v>
+        <v>58</v>
       </c>
       <c r="B79" t="n">
         <v>2</v>
@@ -8269,7 +7845,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>306</v>
+        <v>261</v>
       </c>
       <c r="B80" t="n">
         <v>2</v>
@@ -8277,7 +7853,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>308</v>
+        <v>60</v>
       </c>
       <c r="B81" t="n">
         <v>2</v>
@@ -8285,7 +7861,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="B82" t="n">
         <v>2</v>
@@ -8293,7 +7869,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B83" t="n">
         <v>2</v>
@@ -8301,7 +7877,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>312</v>
+        <v>63</v>
       </c>
       <c r="B84" t="n">
         <v>2</v>
@@ -8309,7 +7885,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B85" t="n">
         <v>2</v>
@@ -8317,7 +7893,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>314</v>
+        <v>65</v>
       </c>
       <c r="B86" t="n">
         <v>2</v>
@@ -8325,7 +7901,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="B87" t="n">
         <v>2</v>
@@ -8333,7 +7909,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>319</v>
+        <v>67</v>
       </c>
       <c r="B88" t="n">
         <v>2</v>
@@ -8341,7 +7917,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>320</v>
+        <v>69</v>
       </c>
       <c r="B89" t="n">
         <v>2</v>
@@ -8349,7 +7925,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>321</v>
+        <v>70</v>
       </c>
       <c r="B90" t="n">
         <v>2</v>
@@ -8357,7 +7933,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>324</v>
+        <v>267</v>
       </c>
       <c r="B91" t="n">
         <v>2</v>
@@ -8365,7 +7941,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>325</v>
+        <v>71</v>
       </c>
       <c r="B92" t="n">
         <v>2</v>
@@ -8373,7 +7949,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="B93" t="n">
         <v>2</v>
@@ -8381,7 +7957,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>327</v>
+        <v>276</v>
       </c>
       <c r="B94" t="n">
         <v>2</v>
@@ -8389,7 +7965,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>328</v>
+        <v>73</v>
       </c>
       <c r="B95" t="n">
         <v>2</v>
@@ -8397,7 +7973,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="B96" t="n">
         <v>2</v>
@@ -8405,7 +7981,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>329</v>
+        <v>75</v>
       </c>
       <c r="B97" t="n">
         <v>2</v>
@@ -8413,7 +7989,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>330</v>
+        <v>76</v>
       </c>
       <c r="B98" t="n">
         <v>2</v>
@@ -8421,7 +7997,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>331</v>
+        <v>78</v>
       </c>
       <c r="B99" t="n">
         <v>2</v>
@@ -8429,7 +8005,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>332</v>
+        <v>79</v>
       </c>
       <c r="B100" t="n">
         <v>2</v>
@@ -8437,7 +8013,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B101" t="n">
         <v>2</v>
@@ -8445,7 +8021,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>333</v>
+        <v>81</v>
       </c>
       <c r="B102" t="n">
         <v>2</v>
@@ -8453,7 +8029,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>334</v>
+        <v>82</v>
       </c>
       <c r="B103" t="n">
         <v>2</v>
@@ -8461,7 +8037,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>335</v>
+        <v>288</v>
       </c>
       <c r="B104" t="n">
         <v>2</v>
@@ -8469,7 +8045,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="B105" t="n">
         <v>2</v>
@@ -8477,7 +8053,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="B106" t="n">
         <v>2</v>
@@ -8485,7 +8061,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>339</v>
+        <v>83</v>
       </c>
       <c r="B107" t="n">
         <v>2</v>
@@ -8493,7 +8069,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>341</v>
+        <v>84</v>
       </c>
       <c r="B108" t="n">
         <v>2</v>
@@ -8501,7 +8077,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>342</v>
+        <v>85</v>
       </c>
       <c r="B109" t="n">
         <v>2</v>
@@ -8509,7 +8085,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>343</v>
+        <v>86</v>
       </c>
       <c r="B110" t="n">
         <v>2</v>
@@ -8517,7 +8093,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>345</v>
+        <v>300</v>
       </c>
       <c r="B111" t="n">
         <v>2</v>
@@ -8525,7 +8101,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="B112" t="n">
         <v>2</v>
@@ -8533,7 +8109,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>347</v>
+        <v>87</v>
       </c>
       <c r="B113" t="n">
         <v>2</v>
@@ -8541,7 +8117,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>348</v>
+        <v>88</v>
       </c>
       <c r="B114" t="n">
         <v>2</v>
@@ -8549,7 +8125,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>349</v>
+        <v>303</v>
       </c>
       <c r="B115" t="n">
         <v>2</v>
@@ -8557,7 +8133,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>351</v>
+        <v>89</v>
       </c>
       <c r="B116" t="n">
         <v>2</v>
@@ -8565,7 +8141,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>352</v>
+        <v>305</v>
       </c>
       <c r="B117" t="n">
         <v>2</v>
@@ -8573,7 +8149,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>353</v>
+        <v>90</v>
       </c>
       <c r="B118" t="n">
         <v>2</v>
@@ -8581,7 +8157,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>354</v>
+        <v>307</v>
       </c>
       <c r="B119" t="n">
         <v>2</v>
@@ -8589,7 +8165,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>355</v>
+        <v>91</v>
       </c>
       <c r="B120" t="n">
         <v>2</v>
@@ -8597,7 +8173,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>356</v>
+        <v>93</v>
       </c>
       <c r="B121" t="n">
         <v>2</v>
@@ -8605,7 +8181,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>124</v>
+        <v>309</v>
       </c>
       <c r="B122" t="n">
         <v>2</v>
@@ -8613,7 +8189,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>128</v>
+        <v>310</v>
       </c>
       <c r="B123" t="n">
         <v>2</v>
@@ -8621,7 +8197,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>357</v>
+        <v>313</v>
       </c>
       <c r="B124" t="n">
         <v>2</v>
@@ -8629,7 +8205,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>360</v>
+        <v>315</v>
       </c>
       <c r="B125" t="n">
         <v>2</v>
@@ -8637,7 +8213,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>316</v>
       </c>
       <c r="B126" t="n">
         <v>2</v>
@@ -8645,7 +8221,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>362</v>
+        <v>96</v>
       </c>
       <c r="B127" t="n">
         <v>2</v>
@@ -8653,7 +8229,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>363</v>
+        <v>97</v>
       </c>
       <c r="B128" t="n">
         <v>2</v>
@@ -8661,7 +8237,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>364</v>
+        <v>98</v>
       </c>
       <c r="B129" t="n">
         <v>2</v>
@@ -8669,7 +8245,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>366</v>
+        <v>317</v>
       </c>
       <c r="B130" t="n">
         <v>2</v>
@@ -8677,7 +8253,7 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="B131" t="n">
         <v>2</v>
@@ -8685,7 +8261,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>369</v>
+        <v>99</v>
       </c>
       <c r="B132" t="n">
         <v>2</v>
@@ -8693,7 +8269,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>370</v>
+        <v>100</v>
       </c>
       <c r="B133" t="n">
         <v>2</v>
@@ -8701,7 +8277,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="B134" t="n">
         <v>2</v>
@@ -8709,7 +8285,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>372</v>
+        <v>102</v>
       </c>
       <c r="B135" t="n">
         <v>2</v>
@@ -8717,7 +8293,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>373</v>
+        <v>322</v>
       </c>
       <c r="B136" t="n">
         <v>2</v>
@@ -8725,7 +8301,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>374</v>
+        <v>323</v>
       </c>
       <c r="B137" t="n">
         <v>2</v>
@@ -8733,7 +8309,7 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>376</v>
+        <v>103</v>
       </c>
       <c r="B138" t="n">
         <v>2</v>
@@ -8741,7 +8317,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>377</v>
+        <v>104</v>
       </c>
       <c r="B139" t="n">
         <v>2</v>
@@ -8749,7 +8325,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="B140" t="n">
         <v>2</v>
@@ -8757,7 +8333,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>380</v>
+        <v>107</v>
       </c>
       <c r="B141" t="n">
         <v>2</v>
@@ -8765,7 +8341,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>381</v>
+        <v>108</v>
       </c>
       <c r="B142" t="n">
         <v>2</v>
@@ -8773,7 +8349,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>383</v>
+        <v>110</v>
       </c>
       <c r="B143" t="n">
         <v>2</v>
@@ -8781,7 +8357,7 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="B144" t="n">
         <v>2</v>
@@ -8789,7 +8365,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>384</v>
+        <v>112</v>
       </c>
       <c r="B145" t="n">
         <v>2</v>
@@ -8797,7 +8373,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>385</v>
+        <v>338</v>
       </c>
       <c r="B146" t="n">
         <v>2</v>
@@ -8805,7 +8381,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>387</v>
+        <v>113</v>
       </c>
       <c r="B147" t="n">
         <v>2</v>
@@ -8813,7 +8389,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>389</v>
+        <v>340</v>
       </c>
       <c r="B148" t="n">
         <v>2</v>
@@ -8821,7 +8397,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>390</v>
+        <v>114</v>
       </c>
       <c r="B149" t="n">
         <v>2</v>
@@ -8829,7 +8405,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>391</v>
+        <v>115</v>
       </c>
       <c r="B150" t="n">
         <v>2</v>
@@ -8837,7 +8413,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>146</v>
+        <v>344</v>
       </c>
       <c r="B151" t="n">
         <v>2</v>
@@ -8845,7 +8421,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>395</v>
+        <v>116</v>
       </c>
       <c r="B152" t="n">
         <v>2</v>
@@ -8853,7 +8429,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>396</v>
+        <v>117</v>
       </c>
       <c r="B153" t="n">
         <v>2</v>
@@ -8861,7 +8437,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="B154" t="n">
         <v>2</v>
@@ -8869,7 +8445,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>397</v>
+        <v>119</v>
       </c>
       <c r="B155" t="n">
         <v>2</v>
@@ -8877,7 +8453,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="B156" t="n">
         <v>2</v>
@@ -8885,7 +8461,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>402</v>
+        <v>350</v>
       </c>
       <c r="B157" t="n">
         <v>2</v>
@@ -8893,7 +8469,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>403</v>
+        <v>121</v>
       </c>
       <c r="B158" t="n">
         <v>2</v>
@@ -8901,7 +8477,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="B159" t="n">
         <v>2</v>
@@ -8909,7 +8485,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>407</v>
+        <v>123</v>
       </c>
       <c r="B160" t="n">
         <v>2</v>
@@ -8917,7 +8493,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>411</v>
+        <v>125</v>
       </c>
       <c r="B161" t="n">
         <v>2</v>
@@ -8925,7 +8501,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B162" t="n">
         <v>2</v>
@@ -8933,7 +8509,7 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B163" t="n">
         <v>2</v>
@@ -8941,7 +8517,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>412</v>
+        <v>129</v>
       </c>
       <c r="B164" t="n">
         <v>2</v>
@@ -8949,7 +8525,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>413</v>
+        <v>358</v>
       </c>
       <c r="B165" t="n">
         <v>2</v>
@@ -8957,7 +8533,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>414</v>
+        <v>359</v>
       </c>
       <c r="B166" t="n">
         <v>2</v>
@@ -8965,7 +8541,7 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>415</v>
+        <v>130</v>
       </c>
       <c r="B167" t="n">
         <v>2</v>
@@ -8973,7 +8549,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>416</v>
+        <v>361</v>
       </c>
       <c r="B168" t="n">
         <v>2</v>
@@ -8981,7 +8557,7 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="B169" t="n">
         <v>2</v>
@@ -8989,7 +8565,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>159</v>
+        <v>367</v>
       </c>
       <c r="B170" t="n">
         <v>2</v>
@@ -8997,7 +8573,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>418</v>
+        <v>371</v>
       </c>
       <c r="B171" t="n">
         <v>2</v>
@@ -9005,7 +8581,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="B172" t="n">
         <v>2</v>
@@ -9013,7 +8589,7 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>421</v>
+        <v>134</v>
       </c>
       <c r="B173" t="n">
         <v>2</v>
@@ -9021,7 +8597,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>422</v>
+        <v>375</v>
       </c>
       <c r="B174" t="n">
         <v>2</v>
@@ -9029,7 +8605,7 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>423</v>
+        <v>378</v>
       </c>
       <c r="B175" t="n">
         <v>2</v>
@@ -9037,7 +8613,7 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>424</v>
+        <v>379</v>
       </c>
       <c r="B176" t="n">
         <v>2</v>
@@ -9045,7 +8621,7 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="B177" t="n">
         <v>2</v>
@@ -9053,7 +8629,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>426</v>
+        <v>136</v>
       </c>
       <c r="B178" t="n">
         <v>2</v>
@@ -9061,7 +8637,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>427</v>
+        <v>137</v>
       </c>
       <c r="B179" t="n">
         <v>2</v>
@@ -9069,7 +8645,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>428</v>
+        <v>138</v>
       </c>
       <c r="B180" t="n">
         <v>2</v>
@@ -9077,7 +8653,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>429</v>
+        <v>139</v>
       </c>
       <c r="B181" t="n">
         <v>2</v>
@@ -9085,7 +8661,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B182" t="n">
         <v>2</v>
@@ -9093,7 +8669,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>430</v>
+        <v>142</v>
       </c>
       <c r="B183" t="n">
         <v>2</v>
@@ -9101,7 +8677,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>433</v>
+        <v>386</v>
       </c>
       <c r="B184" t="n">
         <v>2</v>
@@ -9109,7 +8685,7 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>171</v>
+        <v>388</v>
       </c>
       <c r="B185" t="n">
         <v>2</v>
@@ -9117,7 +8693,7 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>438</v>
+        <v>143</v>
       </c>
       <c r="B186" t="n">
         <v>2</v>
@@ -9125,7 +8701,7 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>439</v>
+        <v>144</v>
       </c>
       <c r="B187" t="n">
         <v>2</v>
@@ -9133,7 +8709,7 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>440</v>
+        <v>145</v>
       </c>
       <c r="B188" t="n">
         <v>2</v>
@@ -9141,7 +8717,7 @@
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>441</v>
+        <v>392</v>
       </c>
       <c r="B189" t="n">
         <v>2</v>
@@ -9149,7 +8725,7 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>442</v>
+        <v>393</v>
       </c>
       <c r="B190" t="n">
         <v>2</v>
@@ -9157,7 +8733,7 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="B191" t="n">
         <v>2</v>
@@ -9165,7 +8741,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>187</v>
+        <v>398</v>
       </c>
       <c r="B192" t="n">
         <v>2</v>
@@ -9173,7 +8749,7 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>445</v>
+        <v>148</v>
       </c>
       <c r="B193" t="n">
         <v>2</v>
@@ -9181,7 +8757,7 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>447</v>
+        <v>399</v>
       </c>
       <c r="B194" t="n">
         <v>2</v>
@@ -9189,7 +8765,7 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>448</v>
+        <v>401</v>
       </c>
       <c r="B195" t="n">
         <v>2</v>
@@ -9197,7 +8773,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>449</v>
+        <v>404</v>
       </c>
       <c r="B196" t="n">
         <v>2</v>
@@ -9205,7 +8781,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>450</v>
+        <v>405</v>
       </c>
       <c r="B197" t="n">
         <v>2</v>
@@ -9213,7 +8789,7 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>451</v>
+        <v>406</v>
       </c>
       <c r="B198" t="n">
         <v>2</v>
@@ -9221,7 +8797,7 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>452</v>
+        <v>150</v>
       </c>
       <c r="B199" t="n">
         <v>2</v>
@@ -9229,7 +8805,7 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>455</v>
+        <v>408</v>
       </c>
       <c r="B200" t="n">
         <v>2</v>
@@ -9237,7 +8813,7 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>457</v>
+        <v>409</v>
       </c>
       <c r="B201" t="n">
         <v>2</v>
@@ -9245,7 +8821,7 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="B202" t="n">
         <v>2</v>
@@ -9253,7 +8829,7 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>458</v>
+        <v>410</v>
       </c>
       <c r="B203" t="n">
         <v>2</v>
@@ -9261,7 +8837,7 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>459</v>
+        <v>153</v>
       </c>
       <c r="B204" t="n">
         <v>2</v>
@@ -9269,7 +8845,7 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>461</v>
+        <v>155</v>
       </c>
       <c r="B205" t="n">
         <v>2</v>
@@ -9277,7 +8853,7 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>462</v>
+        <v>156</v>
       </c>
       <c r="B206" t="n">
         <v>2</v>
@@ -9285,7 +8861,7 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>463</v>
+        <v>157</v>
       </c>
       <c r="B207" t="n">
         <v>2</v>
@@ -9293,9 +8869,433 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>464</v>
+        <v>158</v>
       </c>
       <c r="B208" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>161</v>
+      </c>
+      <c r="B209" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>419</v>
+      </c>
+      <c r="B210" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>162</v>
+      </c>
+      <c r="B212" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>163</v>
+      </c>
+      <c r="B213" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>164</v>
+      </c>
+      <c r="B214" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>165</v>
+      </c>
+      <c r="B215" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>166</v>
+      </c>
+      <c r="B216" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>168</v>
+      </c>
+      <c r="B217" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>431</v>
+      </c>
+      <c r="B218" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>432</v>
+      </c>
+      <c r="B219" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>169</v>
+      </c>
+      <c r="B220" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>434</v>
+      </c>
+      <c r="B221" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>170</v>
+      </c>
+      <c r="B222" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>435</v>
+      </c>
+      <c r="B223" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>172</v>
+      </c>
+      <c r="B224" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>173</v>
+      </c>
+      <c r="B225" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>436</v>
+      </c>
+      <c r="B226" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>174</v>
+      </c>
+      <c r="B227" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>437</v>
+      </c>
+      <c r="B228" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>175</v>
+      </c>
+      <c r="B229" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>176</v>
+      </c>
+      <c r="B230" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>177</v>
+      </c>
+      <c r="B231" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>178</v>
+      </c>
+      <c r="B232" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>179</v>
+      </c>
+      <c r="B233" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>181</v>
+      </c>
+      <c r="B234" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>182</v>
+      </c>
+      <c r="B235" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>183</v>
+      </c>
+      <c r="B236" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>184</v>
+      </c>
+      <c r="B237" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>443</v>
+      </c>
+      <c r="B238" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>185</v>
+      </c>
+      <c r="B239" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>444</v>
+      </c>
+      <c r="B240" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>186</v>
+      </c>
+      <c r="B241" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>446</v>
+      </c>
+      <c r="B242" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>453</v>
+      </c>
+      <c r="B243" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>454</v>
+      </c>
+      <c r="B244" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>456</v>
+      </c>
+      <c r="B245" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>189</v>
+      </c>
+      <c r="B246" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>460</v>
+      </c>
+      <c r="B247" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>190</v>
+      </c>
+      <c r="B248" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>191</v>
+      </c>
+      <c r="B249" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>192</v>
+      </c>
+      <c r="B250" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>193</v>
+      </c>
+      <c r="B251" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>194</v>
+      </c>
+      <c r="B252" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>195</v>
+      </c>
+      <c r="B253" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>196</v>
+      </c>
+      <c r="B254" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>197</v>
+      </c>
+      <c r="B255" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>465</v>
+      </c>
+      <c r="B256" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>466</v>
+      </c>
+      <c r="B257" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>467</v>
+      </c>
+      <c r="B258" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>198</v>
+      </c>
+      <c r="B259" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>199</v>
+      </c>
+      <c r="B260" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>468</v>
+      </c>
+      <c r="B261" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>